<commit_message>
Added an external folder
</commit_message>
<xml_diff>
--- a/database/pokemon_munchkin.xlsx
+++ b/database/pokemon_munchkin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Projects\Card-Generator\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFFEBCF-AEEE-4EBB-8619-B950AF5B0678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7CAA53-CCB9-43BD-B565-91DC50FA4398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{AF3255ED-308E-414A-97A8-9EF8AC8300DD}"/>
   </bookViews>
@@ -71,11 +71,6 @@
     <t>Venusaur</t>
   </si>
   <si>
-    <t>Starter Rivalry: If fighting alone, gain +3 bonus_x000D_
-Poison Powder: Roll 1d4. Weaken a monster by -x in combat_x000D_
-Chloroblast: Discard 1 treasure card to instantly defeat any monster with a bonus of 15 or lower. Can be used twice if itג€™s sunny outside [G]</t>
-  </si>
-  <si>
     <t>Charmander</t>
   </si>
   <si>
@@ -157,72 +152,37 @@
     <t>Poison, Bug</t>
   </si>
   <si>
-    <t>String Shot: Roll 1d6. On a 4+, the Monsterג€™s bonus is reduced by -2.</t>
-  </si>
-  <si>
     <t>Kakuna</t>
   </si>
   <si>
-    <t>String Shot: Roll 1d6. On a 4+, the Monsterג€™s bonus is reduced by -2_x000D_
-Harden: When you fail to run from a monster, you may roll 1d6. On a 4-, you get half of the penalties rounded down</t>
-  </si>
-  <si>
     <t>Beedrill</t>
   </si>
   <si>
-    <t>String Shot: Roll 1d6. On a 4+, the Monsterג€™s bonus is reduced by -2_x000D_
-Harden: When you fail to run from a monster, you may roll 1d6. On a 4-, you get half of the penalties rounded down_x000D_
-Swarm: Gain +5 bonus if youג€™re not the top 1 player</t>
-  </si>
-  <si>
     <t>Pidgey</t>
   </si>
   <si>
     <t>Normal, Flying</t>
   </si>
   <si>
-    <t>Frisk: Roll 1d6. On a 4+, look at someoneג€™s hand and take a card of your choice</t>
-  </si>
-  <si>
     <t>Pidgeotto</t>
   </si>
   <si>
-    <t>Frisk: Roll 1d6. On a 4+, look at someoneג€™s hand and take a card of your choice_x000D_
-Keen Eye: One of your rolls will get +2. You need to choose the roll beforehand</t>
-  </si>
-  <si>
     <t>Pidgeot</t>
   </si>
   <si>
-    <t>Frisk: Roll 1d6. On a 4+, look at someoneג€™s hand and take a card of your choice_x000D_
-Keen Eye: One of your rolls will get +2. You need to choose the roll beforehand_x000D_
-Hurricane: End a battle [G]</t>
-  </si>
-  <si>
     <t>Rattata</t>
   </si>
   <si>
     <t>Normal</t>
   </si>
   <si>
-    <t>Ratatouille: Mmmmmm foodג€¦ If thereג€™s food on the table, eat some! Then, get +2 for the combat</t>
-  </si>
-  <si>
     <t>Raticate</t>
   </si>
   <si>
-    <t>Ratatouille: Mmmmmm foodג€¦ If thereג€™s food on the table, eat some! Then, get +2 for the combat_x000D_
-Hyper Fang: Roll 1d6. On a 4+, gain +4 bonus for that combat</t>
-  </si>
-  <si>
     <t>Spearow</t>
   </si>
   <si>
     <t>Fearow</t>
-  </si>
-  <si>
-    <t>Frisk: Roll 1d6. On a 4+, look at someoneג€™s hand and take a card of your choice_x000D_
-Fear Row: The row of people sitting in front of you are afraid of you :O They get -2 for the rest of the game</t>
   </si>
   <si>
     <t>Ekans</t>
@@ -247,9 +207,6 @@
     <t>Electric</t>
   </si>
   <si>
-    <t>Mascot: Pikachu! Pikachu! STFU SYBAU TS PMOג€¦ You get +3 bonus. The bonus will be lost if evolved.</t>
-  </si>
-  <si>
     <t>Raichu</t>
   </si>
   <si>
@@ -356,14 +313,7 @@
     <t>Poison, Flying</t>
   </si>
   <si>
-    <t>Supersonic: Roll 1d100. On a 73+, the monster gets confused, and 1/4 of itג€™s bonus is given to the player</t>
-  </si>
-  <si>
     <t>Golbat</t>
-  </si>
-  <si>
-    <t>Supersonic: Roll 1d100. On a 73+, the monster gets confused, and 1/4 of itג€™s bonus is given to the player_x000D_
-Hotel Transylvania: Blablablaג€¦ Suck the blood from a playerג€¦ He loses -3 bonus for the rest of the game [G]</t>
   </si>
   <si>
     <t>Oddish</t>
@@ -406,16 +356,9 @@
     <t>Venonat</t>
   </si>
   <si>
-    <t>Big ahh Eyes: Roll 1d6. On a 2+, look at another playerג€™s hand</t>
-  </si>
-  <si>
     <t>Venomoth</t>
   </si>
   <si>
-    <t>Big ahh Eyes: Roll 1d6. On a 2+, look at another playerג€™s hand_x000D_
-See The Light: If you die, you get 2 times the cards and a Pokemon. You can choose to die [G]</t>
-  </si>
-  <si>
     <t>Diglett</t>
   </si>
   <si>
@@ -431,16 +374,9 @@
     <t>Meowth</t>
   </si>
   <si>
-    <t>Pay Day: Draw an extra treasure card on win. Canג€™t be parsed into a Pokemon</t>
-  </si>
-  <si>
     <t>Persian</t>
   </si>
   <si>
-    <t>Pay Day: Draw an extra treasure card on win. Canג€™t be parsed into a Pokemon_x000D_
-Pickpocket: Roll 1d4. On a 1, a player steals a card from you. On a 2, nothing happens. On a 3, take a random card from a player. On a 4, choose a card from a player</t>
-  </si>
-  <si>
     <t>Psyduck</t>
   </si>
   <si>
@@ -448,10 +384,6 @@
   </si>
   <si>
     <t>Golduck</t>
-  </si>
-  <si>
-    <t>A duck walked up to a lemonade stand: Force a re-roll. If there is a lemon on the table, you can force twice for the same roll_x000D_
-Quack: Quack! Quack. Quackג€¦ :( (+10 bonus for the combat) [G]</t>
   </si>
   <si>
     <t>Mankey</t>
@@ -473,16 +405,9 @@
     <t>Growlithe</t>
   </si>
   <si>
-    <t>Loyal Companion: You canג€™t lose your Pokemon</t>
-  </si>
-  <si>
     <t>Arcanine</t>
   </si>
   <si>
-    <t>Loyal Companion: You canג€™t lose your Pokemon_x000D_
-Intimidate: All monsters lose -3 bonus in combat</t>
-  </si>
-  <si>
     <t>Poliwag</t>
   </si>
   <si>
@@ -492,19 +417,12 @@
     <t>Poliwhirl</t>
   </si>
   <si>
-    <t>Amphibious: If thereג€™s water near you, gain additional +2 bonus</t>
-  </si>
-  <si>
     <t>Poliwrath</t>
   </si>
   <si>
     <t>Water, Fighting</t>
   </si>
   <si>
-    <t>Amphibious: If thereג€™s water near you, gain additional +2 bonus_x000D_
-Dynamic Punch: Roll 1d6. On a 4+, stun the enemy and reduce their bonus by -4. Else, get confused and lose -1 bonus for this turn</t>
-  </si>
-  <si>
     <t>Abra</t>
   </si>
   <si>
@@ -517,16 +435,7 @@
     <t>Kadabra</t>
   </si>
   <si>
-    <t>Crucio: Roll 1d6. Inflict unbearable pain on the victim. The monster gets -x bonus_x000D_
-Imperio: Roll 1d6. Puts the victim completely under the casterג€™s control. The monster gets +x bonus</t>
-  </si>
-  <si>
     <t>Alakazam</t>
-  </si>
-  <si>
-    <t>Crucio: Roll 1d6. Inflict unbearable pain on the victim. The monster gets -x bonus_x000D_
-Imperio: Roll 1d6. Puts the victim completely under the casterג€™s control. The monster gets +x bonus_x000D_
-Avada Kedavra: Instantly kills the target without causing pain [G]</t>
   </si>
   <si>
     <t>Machop</t>
@@ -594,18 +503,9 @@
     <t>Graveler</t>
   </si>
   <si>
-    <t>Self-Destruct: Kill a monster, but discard the Pokemon [G]_x000D_
-Can you smell what the rock is cooking: If thereג€™s food on the table, you can throw a rock at another player (be wary of the glass table). Give a player -8 bonus [G]</t>
-  </si>
-  <si>
     <t>Golem</t>
   </si>
   <si>
-    <t>Self-Destruct: Kill a monster, but discard the Pokemon [G]_x000D_
-Can you smell what the rock is cooking: If thereג€™s food on the table, you can throw a rock at another player (be wary of the glass table). Give a player -8 bonus [G]_x000D_
-Rock Hard: Gain a shield of +5. If you lose, you can add +5 to the bonus and not win but not lose either</t>
-  </si>
-  <si>
     <t>Ponyta</t>
   </si>
   <si>
@@ -615,24 +515,13 @@
     <t>Rapidash</t>
   </si>
   <si>
-    <t>My Little Pony: You may summon the power of friendship to add +10 to your combat. Can only be used if someone helps you. Everyone must neigh before you play this card [G]_x000D_
-Megan Thee Stallion: Iג€™m a Savage. You are faster than your friends, and if you help them they have to let you choose the treasure you get and get at least half of the treasures</t>
-  </si>
-  <si>
     <t>Slowpoke</t>
   </si>
   <si>
     <t>Water, Psychic</t>
   </si>
   <si>
-    <t>Oblivious: Prevents attraction and intimidate. Your bonus canג€™t go down</t>
-  </si>
-  <si>
     <t>Slowbro</t>
-  </si>
-  <si>
-    <t>Oblivious: Prevents attraction and intimidate. Your bonus canג€™t go down_x000D_
-Curse: Fuck! Shit! Piss! You canג€™t have boots items, but you can carry another big item or another 2 allies</t>
   </si>
   <si>
     <t>Magnemite</t>
@@ -700,10 +589,6 @@
   </si>
   <si>
     <t>Cloyster</t>
-  </si>
-  <si>
-    <t>(:P) : Lick another player! Roll 1d6. The player you licked gets -(x + 1) bonus for the combat_x000D_
-Not Kosher: If thereג€™s a non-kosher food on the table, you gain +3 bonus</t>
   </si>
   <si>
     <t>Gastly</t>
@@ -739,14 +624,7 @@
     <t>Drowzee</t>
   </si>
   <si>
-    <t>Yawner: If a player yawns, he canג€™t fight a monster in his next round</t>
-  </si>
-  <si>
     <t>Hypno</t>
-  </si>
-  <si>
-    <t>Yawner: If a player yawns, he canג€™t fight a monster in his next round_x000D_
-Hypnotize: Your looks hypnotize! Pick a player to help you in combat (canג€™t be used to win the game)</t>
   </si>
   <si>
     <t>Krabby</t>
@@ -793,16 +671,9 @@
     <t>Cubone</t>
   </si>
   <si>
-    <t>Cuboner: If you have boner, thatג€™s weird! If youג€™re a girl, okג€¦ Gain +3 bonus if you have a hand item</t>
-  </si>
-  <si>
     <t>Marowak</t>
   </si>
   <si>
-    <t>Cuboner: If you have boner, thatג€™s weird! If youג€™re a girl, okג€¦ Gain +3 bonus if you have a hand item_x000D_
-Bone Rush: Your bonus is multiplied by x1.5</t>
-  </si>
-  <si>
     <t>Hitmonlee</t>
   </si>
   <si>
@@ -818,9 +689,6 @@
     <t>Lickitung</t>
   </si>
   <si>
-    <t>Lick: Roll a 1d6. On a 4+, lick a player. This player gets paralyzed and needs to roll a 1d6. On a 4+, he is cured. Else, the player canג€™t fight monsters this round</t>
-  </si>
-  <si>
     <t>Koffing</t>
   </si>
   <si>
@@ -836,16 +704,9 @@
     <t>Rhyhorn</t>
   </si>
   <si>
-    <t>Horny: ג€¦ג€¦ג€¦ג€¦ג€¦ג€¦ג€¦ג€¦. If you have a head item, gain additional +2 bonus</t>
-  </si>
-  <si>
     <t>Rhydon</t>
   </si>
   <si>
-    <t>Horny: ג€¦ג€¦ג€¦ג€¦ג€¦ג€¦ג€¦ג€¦. If you have a head item, gain additional +2 bonus
-Rhydon Deez Dih: I have no idea what to put here, I think Iג€™m going to leave this spot empty, Iג€™m going insane making this. Gain +3 bonus</t>
-  </si>
-  <si>
     <t>Chansey</t>
   </si>
   <si>
@@ -870,41 +731,21 @@
     <t>Horsea</t>
   </si>
   <si>
-    <t>Orsi: He is my friend from segel Aram :) Itג€™s funny cause the name of the Pokemon and his name is the same :D Now I have to make Horsea OP somehowג€¦ Gain +3 bonus!</t>
-  </si>
-  <si>
     <t>Seadra</t>
   </si>
   <si>
-    <t>Not Orsi: Well, itג€™s not Orsi nowג€¦ I guess I still need to make it balancedג€¦ Gain the ability to shoot water from your mouth on another player. Roll 1d20. On a 12+, Makes them wet, and they canג€™t fight against monsters they find attractive</t>
-  </si>
-  <si>
     <t>Goldeen</t>
   </si>
   <si>
-    <t>Sushi Material: Letג€™s order from Sushi One! One hour to each direction? Roll 1d100. On 65+, a player canג€™t draw treasures at all this round</t>
-  </si>
-  <si>
     <t>Seaking</t>
   </si>
   <si>
-    <t>Sushi Material: Letג€™s order from Sushi One! One hour to each direction? Roll 1d100. On 65+, a player canג€™t draw treasures at all this round_x000D_
-Namor, King of the Sea: Draw 5 treasures [G]</t>
-  </si>
-  <si>
     <t>Staryu</t>
   </si>
   <si>
-    <t>Patrick Star: You become the star of the match! Each time a player needs to discard cards, you get the cards (only works if youג€™re not the top 1 player)</t>
-  </si>
-  <si>
     <t>Starmie</t>
   </si>
   <si>
-    <t>Patrick Star: You become the star of the match! Each time a player needs to discard cards, you get the cards (only works if youג€™re not the top 1 player)_x000D_
-Starג€¦ Me?: Your card limit is raised by 3</t>
-  </si>
-  <si>
     <t>Mr-Mime</t>
   </si>
   <si>
@@ -926,9 +767,6 @@
     <t>Psychic, Ice</t>
   </si>
   <si>
-    <t>Youג€™re a Jinx!: Jinx a player. This player will get the next 3 curses that any player draws, including cards the cursed player draws [G]</t>
-  </si>
-  <si>
     <t>Electabuzz</t>
   </si>
   <si>
@@ -965,15 +803,9 @@
     <t>Water, Flying</t>
   </si>
   <si>
-    <t>Hyper Beam: You get +5 bonus for this combat, but canג€™t fight a monster in your next round</t>
-  </si>
-  <si>
     <t>Lapras</t>
   </si>
   <si>
-    <t>Perish Song: Roll 1d6, 3 times. If you roll 4+ on all of the rolls, you can end an ongoing fight, win the fight even though you didnג€™t participate, and kill the other players that fought the monster (can be rolled once in a round until succession) [G]</t>
-  </si>
-  <si>
     <t>Ditto</t>
   </si>
   <si>
@@ -987,10 +819,6 @@
   </si>
   <si>
     <t>Vaporeon</t>
-  </si>
-  <si>
-    <t>Charm: Roll 1d6 and discard a card. The x player needs to help you_x000D_
-Hey guys, did you know that in terms of male humanג€¦: If you read the copy pasta aloud you get +6 bonus for this combat [G]</t>
   </si>
   <si>
     <t>Jolteon</t>
@@ -1028,9 +856,6 @@
     <t>Omastar</t>
   </si>
   <si>
-    <t>WTF IS THAT: Roll 1d4. On a 3+, a player canג€™t use their Pokemon for their next combat</t>
-  </si>
-  <si>
     <t>Kabuto</t>
   </si>
   <si>
@@ -1103,9 +928,6 @@
     <t>Mewtwo</t>
   </si>
   <si>
-    <t>MeowTastic: Level-Up (you canג€™t win with this) [G]</t>
-  </si>
-  <si>
     <t>Mew</t>
   </si>
   <si>
@@ -1116,6 +938,184 @@
   </si>
   <si>
     <t>stage</t>
+  </si>
+  <si>
+    <t>Starter Rivalry: If fighting alone, gain +3 bonus_x000D_
+Poison Powder: Roll 1d4. Weaken a monster by -x in combat_x000D_
+Chloroblast: Discard 1 treasure card to instantly defeat any monster with a bonus of 15 or lower. Can be used twice if it's sunny outside [G]</t>
+  </si>
+  <si>
+    <t>String Shot: Roll 1d6. On a 4+, the Monster's bonus is reduced by -2.</t>
+  </si>
+  <si>
+    <t>String Shot: Roll 1d6. On a 4+, the Monster's bonus is reduced by -2_x000D_
+Harden: When you fail to run from a monster, you may roll 1d6. On a 4-, you get half of the penalties rounded down</t>
+  </si>
+  <si>
+    <t>String Shot: Roll 1d6. On a 4+, the Monster's bonus is reduced by -2_x000D_
+Harden: When you fail to run from a monster, you may roll 1d6. On a 4-, you get half of the penalties rounded down_x000D_
+Swarm: Gain +5 bonus if you're not the top 1 player</t>
+  </si>
+  <si>
+    <t>Frisk: Roll 1d6. On a 4+, look at someone's hand and take a card of your choice</t>
+  </si>
+  <si>
+    <t>Frisk: Roll 1d6. On a 4+, look at someone's hand and take a card of your choice_x000D_
+Keen Eye: One of your rolls will get +2. You need to choose the roll beforehand</t>
+  </si>
+  <si>
+    <t>Frisk: Roll 1d6. On a 4+, look at someone's hand and take a card of your choice_x000D_
+Keen Eye: One of your rolls will get +2. You need to choose the roll beforehand_x000D_
+Hurricane: End a battle [G]</t>
+  </si>
+  <si>
+    <t>Frisk: Roll 1d6. On a 4+, look at someone's hand and take a card of your choice_x000D_
+Fear Row: The row of people sitting in front of you are afraid of you :O They get -2 for the rest of the game</t>
+  </si>
+  <si>
+    <t>Supersonic: Roll 1d100. On a 73+, the monster gets confused, and 1/4 of it's bonus is given to the player</t>
+  </si>
+  <si>
+    <t>Big ahh Eyes: Roll 1d6. On a 2+, look at another player's hand</t>
+  </si>
+  <si>
+    <t>Big ahh Eyes: Roll 1d6. On a 2+, look at another player's hand_x000D_
+See The Light: If you die, you get 2 times the cards and a Pokemon. You can choose to die [G]</t>
+  </si>
+  <si>
+    <t>Pay Day: Draw an extra treasure card on win. Can't be parsed into a Pokemon</t>
+  </si>
+  <si>
+    <t>Pay Day: Draw an extra treasure card on win. Can't be parsed into a Pokemon_x000D_
+Pickpocket: Roll 1d4. On a 1, a player steals a card from you. On a 2, nothing happens. On a 3, take a random card from a player. On a 4, choose a card from a player</t>
+  </si>
+  <si>
+    <t>Loyal Companion: You can't lose your Pokemon</t>
+  </si>
+  <si>
+    <t>Loyal Companion: You can't lose your Pokemon_x000D_
+Intimidate: All monsters lose -3 bonus in combat</t>
+  </si>
+  <si>
+    <t>Amphibious: If there's water near you, gain additional +2 bonus</t>
+  </si>
+  <si>
+    <t>Amphibious: If there's water near you, gain additional +2 bonus_x000D_
+Dynamic Punch: Roll 1d6. On a 4+, stun the enemy and reduce their bonus by -4. Else, get confused and lose -1 bonus for this turn</t>
+  </si>
+  <si>
+    <t>Crucio: Roll 1d6. Inflict unbearable pain on the victim. The monster gets -x bonus_x000D_
+Imperio: Roll 1d6. Puts the victim completely under the caster's control. The monster gets +x bonus</t>
+  </si>
+  <si>
+    <t>Crucio: Roll 1d6. Inflict unbearable pain on the victim. The monster gets -x bonus_x000D_
+Imperio: Roll 1d6. Puts the victim completely under the caster's control. The monster gets +x bonus_x000D_
+Avada Kedavra: Instantly kills the target without causing pain [G]</t>
+  </si>
+  <si>
+    <t>Self-Destruct: Kill a monster, but discard the Pokemon [G]_x000D_
+Can you smell what the rock is cooking: If there's food on the table, you can throw a rock at another player (be wary of the glass table). Give a player -8 bonus [G]</t>
+  </si>
+  <si>
+    <t>Self-Destruct: Kill a monster, but discard the Pokemon [G]_x000D_
+Can you smell what the rock is cooking: If there's food on the table, you can throw a rock at another player (be wary of the glass table). Give a player -8 bonus [G]_x000D_
+Rock Hard: Gain a shield of +5. If you lose, you can add +5 to the bonus and not win but not lose either</t>
+  </si>
+  <si>
+    <t>My Little Pony: You may summon the power of friendship to add +10 to your combat. Can only be used if someone helps you. Everyone must neigh before you play this card [G]_x000D_
+Megan Thee Stallion: I'm a Savage. You are faster than your friends, and if you help them they have to let you choose the treasure you get and get at least half of the treasures</t>
+  </si>
+  <si>
+    <t>Oblivious: Prevents attraction and intimidate. Your bonus can't go down</t>
+  </si>
+  <si>
+    <t>Oblivious: Prevents attraction and intimidate. Your bonus can't go down_x000D_
+Curse: Fuck! Shit! Piss! You can't have boots items, but you can carry another big item or another 2 allies</t>
+  </si>
+  <si>
+    <t>(:P) : Lick another player! Roll 1d6. The player you licked gets -(x + 1) bonus for the combat_x000D_
+Not Kosher: If there's a non-kosher food on the table, you gain +3 bonus</t>
+  </si>
+  <si>
+    <t>Yawner: If a player yawns, he can't fight a monster in his next round</t>
+  </si>
+  <si>
+    <t>Yawner: If a player yawns, he can't fight a monster in his next round_x000D_
+Hypnotize: Your looks hypnotize! Pick a player to help you in combat (can't be used to win the game)</t>
+  </si>
+  <si>
+    <t>Lick: Roll a 1d6. On a 4+, lick a player. This player gets paralyzed and needs to roll a 1d6. On a 4+, he is cured. Else, the player can't fight monsters this round</t>
+  </si>
+  <si>
+    <t>Sushi Material: Let's order from Sushi One! One hour to each direction? Roll 1d100. On 65+, a player can't draw treasures at all this round</t>
+  </si>
+  <si>
+    <t>Sushi Material: Let's order from Sushi One! One hour to each direction? Roll 1d100. On 65+, a player can't draw treasures at all this round_x000D_
+Namor, King of the Sea: Draw 5 treasures [G]</t>
+  </si>
+  <si>
+    <t>Patrick Star: You become the star of the match! Each time a player needs to discard cards, you get the cards (only works if you're not the top 1 player)</t>
+  </si>
+  <si>
+    <t>You're a Jinx!: Jinx a player. This player will get the next 3 curses that any player draws, including cards the cursed player draws [G]</t>
+  </si>
+  <si>
+    <t>Hyper Beam: You get +5 bonus for this combat, but can't fight a monster in your next round</t>
+  </si>
+  <si>
+    <t>Perish Song: Roll 1d6, 3 times. If you roll 4+ on all of the rolls, you can end an ongoing fight, win the fight even though you didn't participate, and kill the other players that fought the monster (can be rolled once in a round until succession) [G]</t>
+  </si>
+  <si>
+    <t>WTF IS THAT: Roll 1d4. On a 3+, a player can't use their Pokemon for their next combat</t>
+  </si>
+  <si>
+    <t>MeowTastic: Level-Up (you can't win with this) [G]</t>
+  </si>
+  <si>
+    <t>Ratatouille: Mmmmmm food... If there's food on the table, eat some! Then, get +2 for the combat</t>
+  </si>
+  <si>
+    <t>Ratatouille: Mmmmmm food... If there's food on the table, eat some! Then, get +2 for the combat_x000D_
+Hyper Fang: Roll 1d6. On a 4+, gain +4 bonus for that combat</t>
+  </si>
+  <si>
+    <t>Mascot: Pikachu! Pikachu! STFU SYBAU TS PMO... You get +3 bonus. The bonus will be lost if evolved.</t>
+  </si>
+  <si>
+    <t>Supersonic: Roll 1d100. On a 73+, the monster gets confused, and 1/4 of it's bonus is given to the player_x000D_
+Hotel Transylvania: Blablabla... Suck the blood from a player... He loses -3 bonus for the rest of the game [G]</t>
+  </si>
+  <si>
+    <t>A duck walked up to a lemonade stand: Force a re-roll. If there is a lemon on the table, you can force twice for the same roll_x000D_
+Quack: Quack! Quack. Quack... :( (+10 bonus for the combat) [G]</t>
+  </si>
+  <si>
+    <t>Cuboner: If you have boner, that's weird! If you're a girl, ok... Gain +3 bonus if you have a hand item</t>
+  </si>
+  <si>
+    <t>Cuboner: If you have boner, that's weird! If you're a girl, ok... Gain +3 bonus if you have a hand item
+Bone Rush: Your bonus is multiplied by x1.5</t>
+  </si>
+  <si>
+    <t>Horny: ......................... If you have a head item, gain additional +2 bonus</t>
+  </si>
+  <si>
+    <t>Horny: ......................... If you have a head item, gain additional +2 bonus
+Rhydon Deez Dih: I have no idea what to put here, I think I'm going to leave this spot empty, I'm going insane making this. Gain +3 bonus</t>
+  </si>
+  <si>
+    <t>Orsi: He is my friend from segel Aram :) It's funny cause the name of the Pokemon and his name is the same :D Now I have to make Horsea OP somehow... Gain +3 bonus!</t>
+  </si>
+  <si>
+    <t>Not Orsi: Well, it's not Orsi now... I guess I still need to make it balanced... Gain the ability to shoot water from your mouth on another player. Roll 1d20. On a 12+, Makes them wet, and they can't fight against monsters they find attractive</t>
+  </si>
+  <si>
+    <t>Patrick Star: You become the star of the match! Each time a player needs to discard cards, you get the cards (only works if you're not the top 1 player)_x000D_
+Star... Me?: Your card limit is raised by 3</t>
+  </si>
+  <si>
+    <t>Charm: Roll 1d6 and discard a card. The x player needs to help you_x000D_
+Hey guys, did you know that in terms of male human...: If you read the copy pasta aloud you get +6 bonus for this combat [G]</t>
   </si>
 </sst>
 </file>
@@ -1981,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24BAFF2-F949-4EFE-AE44-E2730521D7C2}">
   <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="J18" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -2004,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>344</v>
+        <v>295</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2124,12 +2124,12 @@
         <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -2153,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>12</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -2185,15 +2185,15 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -2217,15 +2217,15 @@
         <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -2249,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>12</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="9" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -2281,15 +2281,15 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -2313,15 +2313,15 @@
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2336,7 +2336,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1">
         <v>100</v>
@@ -2345,15 +2345,15 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -2368,7 +2368,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="1">
         <v>250</v>
@@ -2377,15 +2377,15 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -2400,7 +2400,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1">
         <v>500</v>
@@ -2409,15 +2409,15 @@
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2432,7 +2432,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1">
         <v>100</v>
@@ -2441,15 +2441,15 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>41</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -2464,7 +2464,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1">
         <v>250</v>
@@ -2473,15 +2473,15 @@
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>43</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="54" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -2496,7 +2496,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="1">
         <v>500</v>
@@ -2505,15 +2505,15 @@
         <v>2</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>45</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -2528,7 +2528,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="1">
         <v>200</v>
@@ -2537,15 +2537,15 @@
         <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>48</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
@@ -2560,7 +2560,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1">
         <v>450</v>
@@ -2569,15 +2569,15 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>50</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="54" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
@@ -2592,7 +2592,7 @@
         <v>18</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="1">
         <v>700</v>
@@ -2601,15 +2601,15 @@
         <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>52</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -2624,7 +2624,7 @@
         <v>19</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1">
         <v>100</v>
@@ -2633,15 +2633,15 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>55</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -2656,7 +2656,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="1">
         <v>400</v>
@@ -2665,15 +2665,15 @@
         <v>2</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>57</v>
+        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -2688,7 +2688,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="1">
         <v>200</v>
@@ -2697,15 +2697,15 @@
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>48</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
@@ -2720,7 +2720,7 @@
         <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" s="1">
         <v>700</v>
@@ -2729,15 +2729,15 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>60</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -2752,7 +2752,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1">
         <v>250</v>
@@ -2761,15 +2761,15 @@
         <v>1</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -2784,7 +2784,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="1">
         <v>600</v>
@@ -2793,15 +2793,15 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -2816,7 +2816,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="1">
         <v>1000</v>
@@ -2825,15 +2825,15 @@
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>68</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
@@ -2848,7 +2848,7 @@
         <v>26</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="1">
         <v>700</v>
@@ -2857,15 +2857,15 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -2880,7 +2880,7 @@
         <v>27</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" s="1">
         <v>200</v>
@@ -2889,15 +2889,15 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
@@ -2912,7 +2912,7 @@
         <v>28</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29" s="1">
         <v>600</v>
@@ -2921,15 +2921,15 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -2944,7 +2944,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G30" s="1">
         <v>200</v>
@@ -2953,15 +2953,15 @@
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1">
         <v>2</v>
@@ -2976,7 +2976,7 @@
         <v>30</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" s="1">
         <v>400</v>
@@ -2985,15 +2985,15 @@
         <v>2</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1">
         <v>3</v>
@@ -3008,7 +3008,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="1">
         <v>600</v>
@@ -3017,15 +3017,15 @@
         <v>3</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -3040,7 +3040,7 @@
         <v>32</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" s="1">
         <v>200</v>
@@ -3049,15 +3049,15 @@
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B34" s="1">
         <v>2</v>
@@ -3072,7 +3072,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="1">
         <v>400</v>
@@ -3081,15 +3081,15 @@
         <v>2</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B35" s="1">
         <v>3</v>
@@ -3104,7 +3104,7 @@
         <v>34</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G35" s="1">
         <v>600</v>
@@ -3113,15 +3113,15 @@
         <v>3</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -3136,7 +3136,7 @@
         <v>35</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" s="1">
         <v>250</v>
@@ -3145,15 +3145,15 @@
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
@@ -3168,7 +3168,7 @@
         <v>36</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37" s="1">
         <v>600</v>
@@ -3177,15 +3177,15 @@
         <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -3200,7 +3200,7 @@
         <v>37</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38" s="1">
         <v>250</v>
@@ -3209,15 +3209,15 @@
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B39" s="1">
         <v>2</v>
@@ -3232,7 +3232,7 @@
         <v>38</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G39" s="1">
         <v>800</v>
@@ -3241,15 +3241,15 @@
         <v>2</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -3264,7 +3264,7 @@
         <v>39</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G40" s="1">
         <v>300</v>
@@ -3273,15 +3273,15 @@
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B41" s="1">
         <v>2</v>
@@ -3296,7 +3296,7 @@
         <v>40</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G41" s="1">
         <v>650</v>
@@ -3305,15 +3305,15 @@
         <v>2</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -3328,7 +3328,7 @@
         <v>41</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G42" s="1">
         <v>150</v>
@@ -3337,15 +3337,15 @@
         <v>1</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>103</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -3360,7 +3360,7 @@
         <v>42</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G43" s="1">
         <v>350</v>
@@ -3369,15 +3369,15 @@
         <v>2</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>105</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -3392,7 +3392,7 @@
         <v>43</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G44" s="1">
         <v>100</v>
@@ -3404,12 +3404,12 @@
         <v>11</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B45" s="1">
         <v>2</v>
@@ -3424,7 +3424,7 @@
         <v>44</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G45" s="1">
         <v>250</v>
@@ -3436,12 +3436,12 @@
         <v>11</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -3456,7 +3456,7 @@
         <v>45</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G46" s="1">
         <v>500</v>
@@ -3468,12 +3468,12 @@
         <v>11</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -3488,7 +3488,7 @@
         <v>46</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G47" s="1">
         <v>200</v>
@@ -3497,15 +3497,15 @@
         <v>1</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B48" s="1">
         <v>2</v>
@@ -3520,7 +3520,7 @@
         <v>47</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G48" s="1">
         <v>550</v>
@@ -3529,15 +3529,15 @@
         <v>2</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -3552,7 +3552,7 @@
         <v>48</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G49" s="1">
         <v>200</v>
@@ -3561,15 +3561,15 @@
         <v>1</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>118</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B50" s="1">
         <v>2</v>
@@ -3584,7 +3584,7 @@
         <v>49</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G50" s="1">
         <v>500</v>
@@ -3593,15 +3593,15 @@
         <v>2</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>120</v>
+        <v>306</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -3616,7 +3616,7 @@
         <v>50</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G51" s="1">
         <v>250</v>
@@ -3625,15 +3625,15 @@
         <v>1</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B52" s="1">
         <v>2</v>
@@ -3648,7 +3648,7 @@
         <v>51</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G52" s="1">
         <v>750</v>
@@ -3657,15 +3657,15 @@
         <v>2</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -3680,7 +3680,7 @@
         <v>52</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G53" s="1">
         <v>777</v>
@@ -3689,15 +3689,15 @@
         <v>1</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>126</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B54" s="1">
         <v>2</v>
@@ -3712,7 +3712,7 @@
         <v>53</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G54" s="1">
         <v>777</v>
@@ -3721,15 +3721,15 @@
         <v>2</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>128</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -3744,7 +3744,7 @@
         <v>54</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G55" s="1">
         <v>130</v>
@@ -3753,15 +3753,15 @@
         <v>1</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B56" s="1">
         <v>2</v>
@@ -3776,7 +3776,7 @@
         <v>55</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G56" s="1">
         <v>450</v>
@@ -3785,15 +3785,15 @@
         <v>2</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>132</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -3808,7 +3808,7 @@
         <v>56</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G57" s="1">
         <v>200</v>
@@ -3817,15 +3817,15 @@
         <v>1</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B58" s="1">
         <v>2</v>
@@ -3840,7 +3840,7 @@
         <v>57</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G58" s="1">
         <v>600</v>
@@ -3849,15 +3849,15 @@
         <v>2</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B59" s="1">
         <v>1</v>
@@ -3872,7 +3872,7 @@
         <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G59" s="1">
         <v>250</v>
@@ -3881,15 +3881,15 @@
         <v>1</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>139</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B60" s="1">
         <v>2</v>
@@ -3904,7 +3904,7 @@
         <v>59</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G60" s="1">
         <v>750</v>
@@ -3913,15 +3913,15 @@
         <v>2</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>141</v>
+        <v>310</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
@@ -3936,7 +3936,7 @@
         <v>60</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G61" s="1">
         <v>100</v>
@@ -3945,15 +3945,15 @@
         <v>1</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B62" s="1">
         <v>2</v>
@@ -3968,7 +3968,7 @@
         <v>61</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G62" s="1">
         <v>300</v>
@@ -3977,15 +3977,15 @@
         <v>2</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>145</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B63" s="1">
         <v>3</v>
@@ -4000,7 +4000,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G63" s="1">
         <v>500</v>
@@ -4009,15 +4009,15 @@
         <v>3</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>148</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -4032,7 +4032,7 @@
         <v>63</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G64" s="1">
         <v>150</v>
@@ -4041,15 +4041,15 @@
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="B65" s="1">
         <v>2</v>
@@ -4064,7 +4064,7 @@
         <v>64</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G65" s="1">
         <v>400</v>
@@ -4073,15 +4073,15 @@
         <v>2</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>153</v>
+        <v>313</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="54" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="B66" s="1">
         <v>3</v>
@@ -4096,7 +4096,7 @@
         <v>65</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G66" s="1">
         <v>750</v>
@@ -4105,15 +4105,15 @@
         <v>3</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>155</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
@@ -4128,7 +4128,7 @@
         <v>66</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G67" s="1">
         <v>200</v>
@@ -4137,15 +4137,15 @@
         <v>1</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="B68" s="1">
         <v>2</v>
@@ -4160,7 +4160,7 @@
         <v>67</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G68" s="1">
         <v>200</v>
@@ -4169,15 +4169,15 @@
         <v>2</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1">
         <v>3</v>
@@ -4192,7 +4192,7 @@
         <v>68</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G69" s="1">
         <v>800</v>
@@ -4201,15 +4201,15 @@
         <v>3</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
@@ -4224,7 +4224,7 @@
         <v>69</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G70" s="1">
         <v>5</v>
@@ -4236,12 +4236,12 @@
         <v>11</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="B71" s="1">
         <v>2</v>
@@ -4256,7 +4256,7 @@
         <v>70</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G71" s="1">
         <v>10</v>
@@ -4268,12 +4268,12 @@
         <v>11</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1">
         <v>3</v>
@@ -4288,7 +4288,7 @@
         <v>71</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G72" s="1">
         <v>50</v>
@@ -4300,12 +4300,12 @@
         <v>11</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
@@ -4320,7 +4320,7 @@
         <v>72</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G73" s="1">
         <v>400</v>
@@ -4329,15 +4329,15 @@
         <v>1</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B74" s="1">
         <v>2</v>
@@ -4352,7 +4352,7 @@
         <v>73</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G74" s="1">
         <v>800</v>
@@ -4361,15 +4361,15 @@
         <v>2</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -4384,7 +4384,7 @@
         <v>74</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
@@ -4393,15 +4393,15 @@
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B76" s="1">
         <v>2</v>
@@ -4416,7 +4416,7 @@
         <v>75</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G76" s="1">
         <v>0</v>
@@ -4425,15 +4425,15 @@
         <v>2</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>177</v>
+        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="54" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="B77" s="1">
         <v>3</v>
@@ -4448,7 +4448,7 @@
         <v>76</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
@@ -4457,15 +4457,15 @@
         <v>3</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>179</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
@@ -4480,7 +4480,7 @@
         <v>77</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G78" s="1">
         <v>500</v>
@@ -4489,15 +4489,15 @@
         <v>1</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="B79" s="1">
         <v>2</v>
@@ -4512,7 +4512,7 @@
         <v>78</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G79" s="1">
         <v>1000</v>
@@ -4521,15 +4521,15 @@
         <v>2</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>183</v>
+        <v>317</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="B80" s="1">
         <v>1</v>
@@ -4544,7 +4544,7 @@
         <v>79</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G80" s="1">
         <v>200</v>
@@ -4553,15 +4553,15 @@
         <v>1</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>186</v>
+        <v>318</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="B81" s="1">
         <v>2</v>
@@ -4576,7 +4576,7 @@
         <v>80</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G81" s="1">
         <v>800</v>
@@ -4585,15 +4585,15 @@
         <v>2</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
@@ -4608,7 +4608,7 @@
         <v>81</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G82" s="1">
         <v>300</v>
@@ -4617,15 +4617,15 @@
         <v>1</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B83" s="1">
         <v>2</v>
@@ -4640,7 +4640,7 @@
         <v>82</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G83" s="1">
         <v>900</v>
@@ -4649,15 +4649,15 @@
         <v>2</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="B84" s="1">
         <v>1</v>
@@ -4672,7 +4672,7 @@
         <v>83</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G84" s="1">
         <v>150</v>
@@ -4681,15 +4681,15 @@
         <v>1</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
@@ -4704,7 +4704,7 @@
         <v>84</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G85" s="1">
         <v>250</v>
@@ -4713,15 +4713,15 @@
         <v>1</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="B86" s="1">
         <v>2</v>
@@ -4736,7 +4736,7 @@
         <v>85</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G86" s="1">
         <v>750</v>
@@ -4745,15 +4745,15 @@
         <v>2</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="B87" s="1">
         <v>1</v>
@@ -4768,7 +4768,7 @@
         <v>86</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G87" s="1">
         <v>250</v>
@@ -4777,15 +4777,15 @@
         <v>1</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="B88" s="1">
         <v>2</v>
@@ -4800,7 +4800,7 @@
         <v>87</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G88" s="1">
         <v>500</v>
@@ -4809,15 +4809,15 @@
         <v>2</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="B89" s="1">
         <v>1</v>
@@ -4832,7 +4832,7 @@
         <v>88</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G89" s="1">
         <v>-100</v>
@@ -4841,15 +4841,15 @@
         <v>1</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="B90" s="1">
         <v>2</v>
@@ -4864,7 +4864,7 @@
         <v>89</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G90" s="1">
         <v>-500</v>
@@ -4873,15 +4873,15 @@
         <v>2</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="B91" s="1">
         <v>1</v>
@@ -4896,7 +4896,7 @@
         <v>90</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G91" s="1">
         <v>1000</v>
@@ -4905,15 +4905,15 @@
         <v>1</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="B92" s="1">
         <v>2</v>
@@ -4928,7 +4928,7 @@
         <v>91</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G92" s="1">
         <v>1000</v>
@@ -4937,15 +4937,15 @@
         <v>2</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>211</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="B93" s="1">
         <v>1</v>
@@ -4960,7 +4960,7 @@
         <v>92</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G93" s="1">
         <v>100</v>
@@ -4969,15 +4969,15 @@
         <v>1</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="B94" s="1">
         <v>2</v>
@@ -4992,7 +4992,7 @@
         <v>93</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G94" s="1">
         <v>400</v>
@@ -5001,15 +5001,15 @@
         <v>2</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="B95" s="1">
         <v>3</v>
@@ -5024,7 +5024,7 @@
         <v>94</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G95" s="1">
         <v>800</v>
@@ -5033,15 +5033,15 @@
         <v>3</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B96" s="1">
         <v>1</v>
@@ -5056,7 +5056,7 @@
         <v>95</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
@@ -5065,15 +5065,15 @@
         <v>2</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="B97" s="1">
         <v>1</v>
@@ -5088,7 +5088,7 @@
         <v>96</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G97" s="1">
         <v>250</v>
@@ -5097,15 +5097,15 @@
         <v>1</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>222</v>
+        <v>321</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="B98" s="1">
         <v>2</v>
@@ -5120,7 +5120,7 @@
         <v>97</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G98" s="1">
         <v>700</v>
@@ -5129,15 +5129,15 @@
         <v>2</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>224</v>
+        <v>322</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="B99" s="1">
         <v>1</v>
@@ -5152,7 +5152,7 @@
         <v>98</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G99" s="1">
         <v>250</v>
@@ -5161,15 +5161,15 @@
         <v>1</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="B100" s="1">
         <v>2</v>
@@ -5184,7 +5184,7 @@
         <v>99</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G100" s="1">
         <v>900</v>
@@ -5193,15 +5193,15 @@
         <v>2</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="B101" s="1">
         <v>1</v>
@@ -5216,7 +5216,7 @@
         <v>100</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G101" s="1">
         <v>5</v>
@@ -5225,15 +5225,15 @@
         <v>1</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="B102" s="1">
         <v>2</v>
@@ -5248,7 +5248,7 @@
         <v>101</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G102" s="1">
         <v>500</v>
@@ -5257,15 +5257,15 @@
         <v>2</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="B103" s="1">
         <v>1</v>
@@ -5280,7 +5280,7 @@
         <v>102</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G103" s="1">
         <v>444</v>
@@ -5289,15 +5289,15 @@
         <v>1</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B104" s="1">
         <v>2</v>
@@ -5312,7 +5312,7 @@
         <v>103</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G104" s="1">
         <v>888</v>
@@ -5321,15 +5321,15 @@
         <v>2</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="B105" s="1">
         <v>1</v>
@@ -5344,7 +5344,7 @@
         <v>104</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G105" s="1">
         <v>900</v>
@@ -5353,15 +5353,15 @@
         <v>1</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="B106" s="1">
         <v>2</v>
@@ -5376,7 +5376,7 @@
         <v>105</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G106" s="1">
         <v>900</v>
@@ -5385,15 +5385,15 @@
         <v>2</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>241</v>
+        <v>338</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="B107" s="1">
         <v>1</v>
@@ -5408,7 +5408,7 @@
         <v>106</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G107" s="1">
         <v>500</v>
@@ -5417,15 +5417,15 @@
         <v>2</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B108" s="1">
         <v>2</v>
@@ -5440,7 +5440,7 @@
         <v>107</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G108" s="1">
         <v>500</v>
@@ -5449,15 +5449,15 @@
         <v>2</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="B109" s="1">
         <v>1</v>
@@ -5472,7 +5472,7 @@
         <v>108</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G109" s="1">
         <v>700</v>
@@ -5481,15 +5481,15 @@
         <v>2</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>247</v>
+        <v>323</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="B110" s="1">
         <v>1</v>
@@ -5504,7 +5504,7 @@
         <v>109</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G110" s="1">
         <v>-100</v>
@@ -5513,15 +5513,15 @@
         <v>1</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="B111" s="1">
         <v>2</v>
@@ -5536,7 +5536,7 @@
         <v>110</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G111" s="1">
         <v>-200</v>
@@ -5545,15 +5545,15 @@
         <v>2</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="B112" s="1">
         <v>1</v>
@@ -5568,7 +5568,7 @@
         <v>111</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G112" s="1">
         <v>400</v>
@@ -5577,15 +5577,15 @@
         <v>1</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>253</v>
+        <v>339</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="B113" s="1">
         <v>2</v>
@@ -5600,7 +5600,7 @@
         <v>112</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G113" s="1">
         <v>800</v>
@@ -5609,15 +5609,15 @@
         <v>2</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>255</v>
+        <v>340</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
       <c r="B114" s="1">
         <v>1</v>
@@ -5632,7 +5632,7 @@
         <v>113</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G114" s="1">
         <v>450</v>
@@ -5641,15 +5641,15 @@
         <v>2</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="B115" s="1">
         <v>1</v>
@@ -5664,7 +5664,7 @@
         <v>114</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G115" s="1">
         <v>200</v>
@@ -5673,15 +5673,15 @@
         <v>1</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="B116" s="1">
         <v>1</v>
@@ -5696,7 +5696,7 @@
         <v>115</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G116" s="1">
         <v>900</v>
@@ -5705,15 +5705,15 @@
         <v>2</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="B117" s="1">
         <v>1</v>
@@ -5728,7 +5728,7 @@
         <v>116</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G117" s="1">
         <v>100</v>
@@ -5737,15 +5737,15 @@
         <v>2</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>264</v>
+        <v>341</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="B118" s="1">
         <v>2</v>
@@ -5760,7 +5760,7 @@
         <v>117</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G118" s="1">
         <v>500</v>
@@ -5769,15 +5769,15 @@
         <v>2</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>266</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
       <c r="B119" s="1">
         <v>1</v>
@@ -5792,7 +5792,7 @@
         <v>118</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G119" s="1">
         <v>250</v>
@@ -5801,15 +5801,15 @@
         <v>1</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>268</v>
+        <v>324</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="B120" s="1">
         <v>2</v>
@@ -5824,7 +5824,7 @@
         <v>119</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G120" s="1">
         <v>600</v>
@@ -5833,15 +5833,15 @@
         <v>2</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>270</v>
+        <v>325</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
       <c r="B121" s="1">
         <v>1</v>
@@ -5856,7 +5856,7 @@
         <v>120</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G121" s="1">
         <v>250</v>
@@ -5865,15 +5865,15 @@
         <v>1</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>272</v>
+        <v>326</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="B122" s="1">
         <v>2</v>
@@ -5888,7 +5888,7 @@
         <v>121</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G122" s="1">
         <v>300</v>
@@ -5897,15 +5897,15 @@
         <v>2</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>274</v>
+        <v>343</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="B123" s="1">
         <v>1</v>
@@ -5920,7 +5920,7 @@
         <v>122</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G123" s="1">
         <v>600</v>
@@ -5929,15 +5929,15 @@
         <v>2</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="B124" s="1">
         <v>1</v>
@@ -5952,7 +5952,7 @@
         <v>123</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G124" s="1">
         <v>500</v>
@@ -5961,15 +5961,15 @@
         <v>2</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B125" s="1">
         <v>1</v>
@@ -5984,7 +5984,7 @@
         <v>124</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G125" s="1">
         <v>0</v>
@@ -5993,15 +5993,15 @@
         <v>2</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>282</v>
+        <v>327</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="B126" s="1">
         <v>1</v>
@@ -6016,7 +6016,7 @@
         <v>125</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G126" s="1">
         <v>650</v>
@@ -6025,15 +6025,15 @@
         <v>2</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="B127" s="1">
         <v>1</v>
@@ -6048,7 +6048,7 @@
         <v>126</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G127" s="1">
         <v>650</v>
@@ -6057,15 +6057,15 @@
         <v>2</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>286</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>287</v>
+        <v>243</v>
       </c>
       <c r="B128" s="1">
         <v>1</v>
@@ -6080,7 +6080,7 @@
         <v>127</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G128" s="1">
         <v>600</v>
@@ -6089,15 +6089,15 @@
         <v>2</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
       <c r="B129" s="1">
         <v>1</v>
@@ -6112,7 +6112,7 @@
         <v>128</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G129" s="1">
         <v>500</v>
@@ -6121,15 +6121,15 @@
         <v>2</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>290</v>
+        <v>246</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>291</v>
+        <v>247</v>
       </c>
       <c r="B130" s="1">
         <v>1</v>
@@ -6144,7 +6144,7 @@
         <v>129</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G130" s="1">
         <v>0</v>
@@ -6153,15 +6153,15 @@
         <v>0</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>292</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
       <c r="B131" s="1">
         <v>2</v>
@@ -6176,7 +6176,7 @@
         <v>130</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G131" s="1">
         <v>1000</v>
@@ -6185,15 +6185,15 @@
         <v>2</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>294</v>
+        <v>250</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>295</v>
+        <v>328</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="B132" s="1">
         <v>1</v>
@@ -6208,7 +6208,7 @@
         <v>131</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G132" s="1">
         <v>900</v>
@@ -6217,15 +6217,15 @@
         <v>4</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>298</v>
+        <v>252</v>
       </c>
       <c r="B133" s="1">
         <v>1</v>
@@ -6240,7 +6240,7 @@
         <v>132</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
@@ -6249,15 +6249,15 @@
         <v>0</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>299</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>300</v>
+        <v>254</v>
       </c>
       <c r="B134" s="1">
         <v>1</v>
@@ -6272,7 +6272,7 @@
         <v>133</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G134" s="1">
         <v>1000</v>
@@ -6281,15 +6281,15 @@
         <v>1</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>301</v>
+        <v>255</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>302</v>
+        <v>256</v>
       </c>
       <c r="B135" s="1">
         <v>2</v>
@@ -6304,7 +6304,7 @@
         <v>134</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G135" s="1">
         <v>750</v>
@@ -6313,15 +6313,15 @@
         <v>2</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>304</v>
+        <v>257</v>
       </c>
       <c r="B136" s="1">
         <v>2</v>
@@ -6336,7 +6336,7 @@
         <v>135</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G136" s="1">
         <v>750</v>
@@ -6345,15 +6345,15 @@
         <v>2</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>305</v>
+        <v>258</v>
       </c>
     </row>
     <row r="137" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>306</v>
+        <v>259</v>
       </c>
       <c r="B137" s="1">
         <v>2</v>
@@ -6368,7 +6368,7 @@
         <v>136</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G137" s="1">
         <v>750</v>
@@ -6377,15 +6377,15 @@
         <v>2</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>307</v>
+        <v>260</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>308</v>
+        <v>261</v>
       </c>
       <c r="B138" s="1">
         <v>1</v>
@@ -6400,7 +6400,7 @@
         <v>137</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G138" s="1">
         <v>100</v>
@@ -6409,15 +6409,15 @@
         <v>1</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>310</v>
+        <v>263</v>
       </c>
       <c r="B139" s="1">
         <v>1</v>
@@ -6432,7 +6432,7 @@
         <v>138</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="G139" s="1">
         <v>300</v>
@@ -6441,15 +6441,15 @@
         <v>1</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>312</v>
+        <v>265</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>313</v>
+        <v>266</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>314</v>
+        <v>267</v>
       </c>
       <c r="B140" s="1">
         <v>2</v>
@@ -6464,7 +6464,7 @@
         <v>139</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="G140" s="1">
         <v>600</v>
@@ -6473,15 +6473,15 @@
         <v>2</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>312</v>
+        <v>265</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>316</v>
+        <v>268</v>
       </c>
       <c r="B141" s="1">
         <v>1</v>
@@ -6496,7 +6496,7 @@
         <v>140</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="G141" s="1">
         <v>100</v>
@@ -6505,15 +6505,15 @@
         <v>1</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>312</v>
+        <v>265</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>317</v>
+        <v>269</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>318</v>
+        <v>270</v>
       </c>
       <c r="B142" s="1">
         <v>2</v>
@@ -6528,7 +6528,7 @@
         <v>141</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="G142" s="1">
         <v>700</v>
@@ -6537,15 +6537,15 @@
         <v>2</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>312</v>
+        <v>265</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>319</v>
+        <v>271</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="B143" s="1">
         <v>1</v>
@@ -6560,7 +6560,7 @@
         <v>142</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="G143" s="1">
         <v>900</v>
@@ -6569,15 +6569,15 @@
         <v>3</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="B144" s="1">
         <v>1</v>
@@ -6592,7 +6592,7 @@
         <v>143</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G144" s="1">
         <v>950</v>
@@ -6601,15 +6601,15 @@
         <v>4</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="B145" s="1">
         <v>1</v>
@@ -6624,7 +6624,7 @@
         <v>144</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="G145" s="1">
         <v>1000</v>
@@ -6633,15 +6633,15 @@
         <v>5</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="B146" s="1">
         <v>1</v>
@@ -6656,7 +6656,7 @@
         <v>145</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="G146" s="1">
         <v>1000</v>
@@ -6665,15 +6665,15 @@
         <v>5</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>331</v>
+        <v>283</v>
       </c>
       <c r="B147" s="1">
         <v>1</v>
@@ -6688,7 +6688,7 @@
         <v>146</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="G147" s="1">
         <v>1000</v>
@@ -6697,15 +6697,15 @@
         <v>5</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>332</v>
+        <v>284</v>
       </c>
       <c r="B148" s="1">
         <v>1</v>
@@ -6720,7 +6720,7 @@
         <v>147</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="G148" s="1">
         <v>250</v>
@@ -6729,15 +6729,15 @@
         <v>1</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="B149" s="1">
         <v>2</v>
@@ -6752,7 +6752,7 @@
         <v>148</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="G149" s="1">
         <v>600</v>
@@ -6761,15 +6761,15 @@
         <v>2</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="B150" s="1">
         <v>3</v>
@@ -6784,7 +6784,7 @@
         <v>149</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="G150" s="1">
         <v>1000</v>
@@ -6793,15 +6793,15 @@
         <v>4</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>338</v>
+        <v>290</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="B151" s="1">
         <v>1</v>
@@ -6816,7 +6816,7 @@
         <v>150</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="G151" s="1">
         <v>1500</v>
@@ -6825,15 +6825,15 @@
         <v>6</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>341</v>
+        <v>292</v>
       </c>
       <c r="B152" s="1">
         <v>1</v>
@@ -6848,7 +6848,7 @@
         <v>151</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="G152" s="1">
         <v>1750</v>
@@ -6857,10 +6857,10 @@
         <v>6</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more epic stuff
</commit_message>
<xml_diff>
--- a/database/pokemon_munchkin.xlsx
+++ b/database/pokemon_munchkin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Projects\Card-Generator\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7CAA53-CCB9-43BD-B565-91DC50FA4398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799D2FFC-539E-4E1F-9357-54D246B1E4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{AF3255ED-308E-414A-97A8-9EF8AC8300DD}"/>
   </bookViews>
@@ -362,13 +362,7 @@
     <t>Diglett</t>
   </si>
   <si>
-    <t>Earthquake: Force all players to discard 1 card from their hand. Can be recharged by throwing a 1d6 and landing a 5+ [G]</t>
-  </si>
-  <si>
     <t>Dugtrio</t>
-  </si>
-  <si>
-    <t>Earthquake: Force all players to discard 3 cards from their hand. Can be recharged by throwing a 1d6 and landing a 5+ [G]</t>
   </si>
   <si>
     <t>Meowth</t>
@@ -892,9 +886,6 @@
     <t>Ice, Flying</t>
   </si>
   <si>
-    <t>Wings of Legend: Avoid any negative effect [G]</t>
-  </si>
-  <si>
     <t>Zapdos</t>
   </si>
   <si>
@@ -932,9 +923,6 @@
   </si>
   <si>
     <t>Mythical</t>
-  </si>
-  <si>
-    <t>MewTastic: Level-Up (you can win with this) [G]</t>
   </si>
   <si>
     <t>stage</t>
@@ -1069,9 +1057,6 @@
     <t>WTF IS THAT: Roll 1d4. On a 3+, a player can't use their Pokemon for their next combat</t>
   </si>
   <si>
-    <t>MeowTastic: Level-Up (you can't win with this) [G]</t>
-  </si>
-  <si>
     <t>Ratatouille: Mmmmmm food... If there's food on the table, eat some! Then, get +2 for the combat</t>
   </si>
   <si>
@@ -1086,10 +1071,6 @@
 Hotel Transylvania: Blablabla... Suck the blood from a player... He loses -3 bonus for the rest of the game [G]</t>
   </si>
   <si>
-    <t>A duck walked up to a lemonade stand: Force a re-roll. If there is a lemon on the table, you can force twice for the same roll_x000D_
-Quack: Quack! Quack. Quack... :( (+10 bonus for the combat) [G]</t>
-  </si>
-  <si>
     <t>Cuboner: If you have boner, that's weird! If you're a girl, ok... Gain +3 bonus if you have a hand item</t>
   </si>
   <si>
@@ -1116,6 +1097,25 @@
   <si>
     <t>Charm: Roll 1d6 and discard a card. The x player needs to help you_x000D_
 Hey guys, did you know that in terms of male human...: If you read the copy pasta aloud you get +6 bonus for this combat [G]</t>
+  </si>
+  <si>
+    <t>MewTastic: You can win on any Level-up</t>
+  </si>
+  <si>
+    <t>Psystrike: Control a player's entire round (No selling and discarding cards) [G]</t>
+  </si>
+  <si>
+    <t>A duck walked up to a lemonade stand: Force a re-roll. If there is a lemon on the table, you can force twice for the same roll
+Quack: Quack! Quack. Quack... :( (+10 bonus for the combat) [G]</t>
+  </si>
+  <si>
+    <t>Earthquake: Force all players to discard 3 cards from their hand. Can be recharged by throwing a 1d6 once and landing a 6 [G]</t>
+  </si>
+  <si>
+    <t>Earthquake: Force all players to discard 1 card from their hand. Can be recharged by throwing a 1d6 once and landing a 6 [G]</t>
+  </si>
+  <si>
+    <t>Birds of a Feather: Avoid any negative effect. A negative effect can be anything that goes against you [G]</t>
   </si>
 </sst>
 </file>
@@ -1981,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24BAFF2-F949-4EFE-AE44-E2730521D7C2}">
   <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="E141" workbookViewId="0">
+      <selection activeCell="J155" sqref="J155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -2004,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2124,7 +2124,7 @@
         <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -2444,7 +2444,7 @@
         <v>39</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
@@ -2476,7 +2476,7 @@
         <v>39</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="54" x14ac:dyDescent="0.35">
@@ -2508,7 +2508,7 @@
         <v>39</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -2540,7 +2540,7 @@
         <v>43</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
@@ -2572,7 +2572,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="54" x14ac:dyDescent="0.35">
@@ -2604,7 +2604,7 @@
         <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -2636,7 +2636,7 @@
         <v>47</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
@@ -2668,7 +2668,7 @@
         <v>47</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -2700,7 +2700,7 @@
         <v>43</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
@@ -2732,7 +2732,7 @@
         <v>43</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2828,7 +2828,7 @@
         <v>57</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -3340,10 +3340,10 @@
         <v>91</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>92</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>91</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -3564,10 +3564,10 @@
         <v>39</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>39</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -3628,12 +3628,12 @@
         <v>61</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>107</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="1">
         <v>2</v>
@@ -3660,12 +3660,12 @@
         <v>61</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>109</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -3692,12 +3692,12 @@
         <v>47</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B54" s="1">
         <v>2</v>
@@ -3724,12 +3724,12 @@
         <v>47</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -3756,12 +3756,12 @@
         <v>24</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B56" s="1">
         <v>2</v>
@@ -3788,12 +3788,12 @@
         <v>24</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -3817,15 +3817,15 @@
         <v>1</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="1">
         <v>2</v>
@@ -3849,15 +3849,15 @@
         <v>2</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B59" s="1">
         <v>1</v>
@@ -3884,12 +3884,12 @@
         <v>17</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B60" s="1">
         <v>2</v>
@@ -3916,12 +3916,12 @@
         <v>17</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
@@ -3948,12 +3948,12 @@
         <v>24</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B62" s="1">
         <v>2</v>
@@ -3980,12 +3980,12 @@
         <v>24</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B63" s="1">
         <v>3</v>
@@ -4009,15 +4009,15 @@
         <v>3</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -4041,15 +4041,15 @@
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1">
         <v>2</v>
@@ -4073,15 +4073,15 @@
         <v>2</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="54" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" s="1">
         <v>3</v>
@@ -4105,15 +4105,15 @@
         <v>3</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
@@ -4137,15 +4137,15 @@
         <v>1</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B68" s="1">
         <v>2</v>
@@ -4169,15 +4169,15 @@
         <v>2</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B69" s="1">
         <v>3</v>
@@ -4201,15 +4201,15 @@
         <v>3</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
@@ -4236,12 +4236,12 @@
         <v>11</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" s="1">
         <v>2</v>
@@ -4268,12 +4268,12 @@
         <v>11</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" s="1">
         <v>3</v>
@@ -4300,12 +4300,12 @@
         <v>11</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
@@ -4329,15 +4329,15 @@
         <v>1</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B74" s="1">
         <v>2</v>
@@ -4361,15 +4361,15 @@
         <v>2</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -4393,15 +4393,15 @@
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B76" s="1">
         <v>2</v>
@@ -4425,15 +4425,15 @@
         <v>2</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="54" x14ac:dyDescent="0.35">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B77" s="1">
         <v>3</v>
@@ -4457,15 +4457,15 @@
         <v>3</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
@@ -4492,12 +4492,12 @@
         <v>17</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B79" s="1">
         <v>2</v>
@@ -4524,12 +4524,12 @@
         <v>17</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B80" s="1">
         <v>1</v>
@@ -4553,15 +4553,15 @@
         <v>1</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B81" s="1">
         <v>2</v>
@@ -4585,15 +4585,15 @@
         <v>2</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
@@ -4617,15 +4617,15 @@
         <v>1</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B83" s="1">
         <v>2</v>
@@ -4649,15 +4649,15 @@
         <v>2</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B84" s="1">
         <v>1</v>
@@ -4684,12 +4684,12 @@
         <v>43</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
@@ -4716,12 +4716,12 @@
         <v>43</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B86" s="1">
         <v>2</v>
@@ -4748,12 +4748,12 @@
         <v>43</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B87" s="1">
         <v>1</v>
@@ -4780,12 +4780,12 @@
         <v>24</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B88" s="1">
         <v>2</v>
@@ -4809,15 +4809,15 @@
         <v>2</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B89" s="1">
         <v>1</v>
@@ -4844,12 +4844,12 @@
         <v>52</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B90" s="1">
         <v>2</v>
@@ -4876,12 +4876,12 @@
         <v>52</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B91" s="1">
         <v>1</v>
@@ -4908,12 +4908,12 @@
         <v>24</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B92" s="1">
         <v>2</v>
@@ -4937,15 +4937,15 @@
         <v>2</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B93" s="1">
         <v>1</v>
@@ -4969,15 +4969,15 @@
         <v>1</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B94" s="1">
         <v>2</v>
@@ -5001,15 +5001,15 @@
         <v>2</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B95" s="1">
         <v>3</v>
@@ -5033,15 +5033,15 @@
         <v>3</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B96" s="1">
         <v>1</v>
@@ -5065,15 +5065,15 @@
         <v>2</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B97" s="1">
         <v>1</v>
@@ -5097,15 +5097,15 @@
         <v>1</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1">
         <v>2</v>
@@ -5129,15 +5129,15 @@
         <v>2</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B99" s="1">
         <v>1</v>
@@ -5164,12 +5164,12 @@
         <v>24</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B100" s="1">
         <v>2</v>
@@ -5196,12 +5196,12 @@
         <v>24</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B101" s="1">
         <v>1</v>
@@ -5228,12 +5228,12 @@
         <v>57</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B102" s="1">
         <v>2</v>
@@ -5260,12 +5260,12 @@
         <v>57</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B103" s="1">
         <v>1</v>
@@ -5289,15 +5289,15 @@
         <v>1</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B104" s="1">
         <v>2</v>
@@ -5321,15 +5321,15 @@
         <v>2</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B105" s="1">
         <v>1</v>
@@ -5356,12 +5356,12 @@
         <v>61</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B106" s="1">
         <v>2</v>
@@ -5388,12 +5388,12 @@
         <v>61</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B107" s="1">
         <v>1</v>
@@ -5417,15 +5417,15 @@
         <v>2</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B108" s="1">
         <v>2</v>
@@ -5449,15 +5449,15 @@
         <v>2</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B109" s="1">
         <v>1</v>
@@ -5484,12 +5484,12 @@
         <v>47</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B110" s="1">
         <v>1</v>
@@ -5516,12 +5516,12 @@
         <v>52</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B111" s="1">
         <v>2</v>
@@ -5548,12 +5548,12 @@
         <v>52</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B112" s="1">
         <v>1</v>
@@ -5577,15 +5577,15 @@
         <v>1</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B113" s="1">
         <v>2</v>
@@ -5609,15 +5609,15 @@
         <v>2</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B114" s="1">
         <v>1</v>
@@ -5644,12 +5644,12 @@
         <v>47</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B115" s="1">
         <v>1</v>
@@ -5673,15 +5673,15 @@
         <v>1</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B116" s="1">
         <v>1</v>
@@ -5708,12 +5708,12 @@
         <v>47</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B117" s="1">
         <v>1</v>
@@ -5740,12 +5740,12 @@
         <v>24</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B118" s="1">
         <v>2</v>
@@ -5772,12 +5772,12 @@
         <v>24</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B119" s="1">
         <v>1</v>
@@ -5804,12 +5804,12 @@
         <v>24</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B120" s="1">
         <v>2</v>
@@ -5836,12 +5836,12 @@
         <v>24</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B121" s="1">
         <v>1</v>
@@ -5868,12 +5868,12 @@
         <v>24</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="40.5" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B122" s="1">
         <v>2</v>
@@ -5897,15 +5897,15 @@
         <v>2</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B123" s="1">
         <v>1</v>
@@ -5929,15 +5929,15 @@
         <v>2</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B124" s="1">
         <v>1</v>
@@ -5964,12 +5964,12 @@
         <v>36</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B125" s="1">
         <v>1</v>
@@ -5993,15 +5993,15 @@
         <v>2</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B126" s="1">
         <v>1</v>
@@ -6028,12 +6028,12 @@
         <v>57</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B127" s="1">
         <v>1</v>
@@ -6060,12 +6060,12 @@
         <v>17</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B128" s="1">
         <v>1</v>
@@ -6092,12 +6092,12 @@
         <v>31</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B129" s="1">
         <v>1</v>
@@ -6124,12 +6124,12 @@
         <v>47</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B130" s="1">
         <v>1</v>
@@ -6156,12 +6156,12 @@
         <v>24</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B131" s="1">
         <v>2</v>
@@ -6185,15 +6185,15 @@
         <v>2</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B132" s="1">
         <v>1</v>
@@ -6217,15 +6217,15 @@
         <v>4</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B133" s="1">
         <v>1</v>
@@ -6252,12 +6252,12 @@
         <v>47</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B134" s="1">
         <v>1</v>
@@ -6284,12 +6284,12 @@
         <v>47</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B135" s="1">
         <v>2</v>
@@ -6316,12 +6316,12 @@
         <v>24</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B136" s="1">
         <v>2</v>
@@ -6348,12 +6348,12 @@
         <v>57</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B137" s="1">
         <v>2</v>
@@ -6380,12 +6380,12 @@
         <v>17</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B138" s="1">
         <v>1</v>
@@ -6412,12 +6412,12 @@
         <v>47</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B139" s="1">
         <v>1</v>
@@ -6432,7 +6432,7 @@
         <v>138</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G139" s="1">
         <v>300</v>
@@ -6441,15 +6441,15 @@
         <v>1</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B140" s="1">
         <v>2</v>
@@ -6464,7 +6464,7 @@
         <v>139</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G140" s="1">
         <v>600</v>
@@ -6473,15 +6473,15 @@
         <v>2</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B141" s="1">
         <v>1</v>
@@ -6496,7 +6496,7 @@
         <v>140</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G141" s="1">
         <v>100</v>
@@ -6505,15 +6505,15 @@
         <v>1</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B142" s="1">
         <v>2</v>
@@ -6528,7 +6528,7 @@
         <v>141</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G142" s="1">
         <v>700</v>
@@ -6537,15 +6537,15 @@
         <v>2</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B143" s="1">
         <v>1</v>
@@ -6560,7 +6560,7 @@
         <v>142</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G143" s="1">
         <v>900</v>
@@ -6569,15 +6569,15 @@
         <v>3</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B144" s="1">
         <v>1</v>
@@ -6604,12 +6604,12 @@
         <v>47</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B145" s="1">
         <v>1</v>
@@ -6624,7 +6624,7 @@
         <v>144</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G145" s="1">
         <v>1000</v>
@@ -6633,15 +6633,15 @@
         <v>5</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B146" s="1">
         <v>1</v>
@@ -6656,7 +6656,7 @@
         <v>145</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G146" s="1">
         <v>1000</v>
@@ -6665,15 +6665,15 @@
         <v>5</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B147" s="1">
         <v>1</v>
@@ -6688,7 +6688,7 @@
         <v>146</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G147" s="1">
         <v>1000</v>
@@ -6700,12 +6700,12 @@
         <v>21</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B148" s="1">
         <v>1</v>
@@ -6720,7 +6720,7 @@
         <v>147</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G148" s="1">
         <v>250</v>
@@ -6729,15 +6729,15 @@
         <v>1</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B149" s="1">
         <v>2</v>
@@ -6752,7 +6752,7 @@
         <v>148</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G149" s="1">
         <v>600</v>
@@ -6761,15 +6761,15 @@
         <v>2</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B150" s="1">
         <v>3</v>
@@ -6784,7 +6784,7 @@
         <v>149</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G150" s="1">
         <v>1000</v>
@@ -6793,15 +6793,15 @@
         <v>4</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B151" s="1">
         <v>1</v>
@@ -6816,7 +6816,7 @@
         <v>150</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G151" s="1">
         <v>1500</v>
@@ -6825,15 +6825,15 @@
         <v>6</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B152" s="1">
         <v>1</v>
@@ -6848,7 +6848,7 @@
         <v>151</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G152" s="1">
         <v>1750</v>
@@ -6857,10 +6857,10 @@
         <v>6</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>294</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>